<commit_message>
Limpiar código: eliminar exportación y cambiar Reservado por Moncurri
</commit_message>
<xml_diff>
--- a/Datos.xlsx
+++ b/Datos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\archivos Exequiel Fontecilla\PYTHON\SOLICITUDES GRAFICAS\Villarica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\python local\Dashboard-inmobiliario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C90C6D-AAB9-43E6-AED6-3BAE8B42DDCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070B6A62-E95D-484C-8E5C-D9907FB34047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -68,9 +68,6 @@
     <t>Stock Ausente</t>
   </si>
   <si>
-    <t>Reservado</t>
-  </si>
-  <si>
     <t>TIPO</t>
   </si>
   <si>
@@ -87,6 +84,9 @@
   </si>
   <si>
     <t>PRECIO</t>
+  </si>
+  <si>
+    <t>Moncurri</t>
   </si>
 </sst>
 </file>
@@ -142,7 +142,7 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -151,7 +151,7 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -564,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,22 +580,22 @@
   <sheetData>
     <row r="1" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>0</v>
@@ -619,7 +619,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F2" s="2">
         <v>3240</v>
@@ -706,7 +706,7 @@
         <v>5</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F5" s="2">
         <v>2754</v>
@@ -735,7 +735,7 @@
         <v>5</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F6" s="2">
         <v>2754</v>
@@ -764,7 +764,7 @@
         <v>2</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F7" s="2">
         <v>3455</v>
@@ -793,7 +793,7 @@
         <v>6</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F8" s="2">
         <v>3654</v>
@@ -851,7 +851,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F10" s="2">
         <v>3491</v>
@@ -880,7 +880,7 @@
         <v>5</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F11" s="2">
         <v>2784</v>
@@ -967,7 +967,7 @@
         <v>2</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F14" s="2">
         <v>3491</v>
@@ -1054,7 +1054,7 @@
         <v>2</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F17" s="2">
         <v>3312</v>
@@ -1199,7 +1199,7 @@
         <v>5</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F22" s="2">
         <v>2810</v>
@@ -1228,7 +1228,7 @@
         <v>5</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F23" s="2">
         <v>2775</v>
@@ -1315,7 +1315,7 @@
         <v>6</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F26" s="2">
         <v>3680</v>
@@ -1344,7 +1344,7 @@
         <v>2</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F27" s="2">
         <v>3312</v>
@@ -1431,7 +1431,7 @@
         <v>2</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F30" s="2">
         <v>3342</v>
@@ -1576,7 +1576,7 @@
         <v>5</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F35" s="2">
         <v>2836</v>
@@ -1634,7 +1634,7 @@
         <v>2</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F37" s="2">
         <v>3404.4</v>
@@ -1721,7 +1721,7 @@
         <v>2</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F40" s="2">
         <v>3342</v>
@@ -1808,7 +1808,7 @@
         <v>2</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F43" s="2">
         <v>3378</v>
@@ -1895,7 +1895,7 @@
         <v>2</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F46" s="2">
         <v>3544.05</v>
@@ -1924,7 +1924,7 @@
         <v>5</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F47" s="2">
         <v>2834.4</v>
@@ -1953,7 +1953,7 @@
         <v>5</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F48" s="2">
         <v>2834.4</v>
@@ -1982,7 +1982,7 @@
         <v>5</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F49" s="2">
         <v>2834.4</v>
@@ -2011,7 +2011,7 @@
         <v>2</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F50" s="2">
         <v>3544.05</v>
@@ -2069,7 +2069,7 @@
         <v>6</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F52" s="2">
         <v>3752</v>
@@ -2098,7 +2098,7 @@
         <v>2</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F53" s="2">
         <v>3378</v>
@@ -2185,7 +2185,7 @@
         <v>2</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F56" s="2">
         <v>3475</v>
@@ -2272,7 +2272,7 @@
         <v>2</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F59" s="2">
         <v>3643.8</v>
@@ -2330,7 +2330,7 @@
         <v>5</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F61" s="2">
         <v>2914.2</v>
@@ -2359,7 +2359,7 @@
         <v>5</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F62" s="2">
         <v>2914.2</v>
@@ -2388,7 +2388,7 @@
         <v>2</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F63" s="2">
         <v>3643.8</v>
@@ -2446,7 +2446,7 @@
         <v>6</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F65" s="2">
         <v>3859</v>
@@ -2475,7 +2475,7 @@
         <v>2</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F66" s="2">
         <v>3475</v>
@@ -2562,7 +2562,7 @@
         <v>2</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F69" s="2">
         <v>3506</v>
@@ -2852,7 +2852,7 @@
         <v>2</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F79" s="2">
         <v>3506</v>
@@ -2939,7 +2939,7 @@
         <v>2</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F82" s="2">
         <v>3573</v>
@@ -3055,7 +3055,7 @@
         <v>5</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F86" s="2">
         <v>2994</v>
@@ -3084,7 +3084,7 @@
         <v>5</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F87" s="2">
         <v>2994</v>
@@ -3113,7 +3113,7 @@
         <v>5</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F88" s="2">
         <v>2994</v>
@@ -3200,7 +3200,7 @@
         <v>6</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F91" s="2">
         <v>3967</v>
@@ -3229,7 +3229,7 @@
         <v>2</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F92" s="2">
         <v>3573</v>
@@ -3316,7 +3316,7 @@
         <v>2</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F95" s="2">
         <v>3603</v>
@@ -3403,7 +3403,7 @@
         <v>2</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F98" s="2">
         <v>3778.7</v>
@@ -3432,7 +3432,7 @@
         <v>5</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F99" s="2">
         <v>3018.7</v>
@@ -3461,7 +3461,7 @@
         <v>5</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F100" s="2">
         <v>3018.7</v>
@@ -3490,7 +3490,7 @@
         <v>5</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F101" s="2">
         <v>3018.7</v>
@@ -3519,7 +3519,7 @@
         <v>2</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F102" s="2">
         <v>3778.7</v>
@@ -3577,7 +3577,7 @@
         <v>6</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F104" s="2">
         <v>4002</v>
@@ -3606,7 +3606,7 @@
         <v>2</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F105" s="2">
         <v>3603</v>

</xml_diff>